<commit_message>
Adjusted absorbance coeff added and relevant methods created. The values when run against eachother (Input: sampling 2_13 Scattering_DF: sampling2_13) doesn't exactly equal zero but this is likely due to the averaging process that we do to get a per scattering volume absorbance coeff.
</commit_message>
<xml_diff>
--- a/Scattering_Data/Scattering_combined_dataframes.xlsx
+++ b/Scattering_Data/Scattering_combined_dataframes.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>Wavelength</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>STDMaterial_18</t>
-  </si>
-  <si>
-    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -651,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1011,65 +1008,6 @@
         <v>275.8496933333333</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7">
-        <v>1000.111</v>
-      </c>
-      <c r="B7">
-        <v>68.44456666666666</v>
-      </c>
-      <c r="C7">
-        <v>42.50425</v>
-      </c>
-      <c r="D7">
-        <v>57.08346</v>
-      </c>
-      <c r="E7">
-        <v>44.26014</v>
-      </c>
-      <c r="F7">
-        <v>30.97146333333333</v>
-      </c>
-      <c r="G7">
-        <v>52.86748</v>
-      </c>
-      <c r="H7">
-        <v>27.57355</v>
-      </c>
-      <c r="I7">
-        <v>29.94484</v>
-      </c>
-      <c r="J7">
-        <v>57.610755</v>
-      </c>
-      <c r="K7">
-        <v>8.605320000000001</v>
-      </c>
-      <c r="L7">
-        <v>24.93896</v>
-      </c>
-      <c r="M7">
-        <v>9.48343</v>
-      </c>
-      <c r="N7">
-        <v>13.611025</v>
-      </c>
-      <c r="O7">
-        <v>51.52733666666666</v>
-      </c>
-      <c r="P7">
-        <v>59.72284</v>
-      </c>
-      <c r="Q7">
-        <v>66.51241</v>
-      </c>
-      <c r="R7">
-        <v>82.38233</v>
-      </c>
-      <c r="S7">
-        <v>31.20573333333333</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1077,7 +1015,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC7"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1977,119 +1915,6 @@
         <v>228.95901</v>
       </c>
     </row>
-    <row r="7" spans="1:55">
-      <c r="A7">
-        <v>1000.111</v>
-      </c>
-      <c r="B7">
-        <v>41.62532</v>
-      </c>
-      <c r="C7">
-        <v>81.50281</v>
-      </c>
-      <c r="D7">
-        <v>82.20556999999999</v>
-      </c>
-      <c r="E7">
-        <v>57.61047</v>
-      </c>
-      <c r="F7">
-        <v>20.54805</v>
-      </c>
-      <c r="G7">
-        <v>49.35423</v>
-      </c>
-      <c r="J7">
-        <v>57.08346</v>
-      </c>
-      <c r="M7">
-        <v>44.26014</v>
-      </c>
-      <c r="N7">
-        <v>71.48875</v>
-      </c>
-      <c r="O7">
-        <v>13.34719</v>
-      </c>
-      <c r="P7">
-        <v>8.07845</v>
-      </c>
-      <c r="R7">
-        <v>52.86748</v>
-      </c>
-      <c r="T7">
-        <v>27.57355</v>
-      </c>
-      <c r="X7">
-        <v>23.00695</v>
-      </c>
-      <c r="Y7">
-        <v>36.88273</v>
-      </c>
-      <c r="Z7">
-        <v>68.15085000000001</v>
-      </c>
-      <c r="AA7">
-        <v>47.07066</v>
-      </c>
-      <c r="AC7">
-        <v>8.605320000000001</v>
-      </c>
-      <c r="AF7">
-        <v>24.93896</v>
-      </c>
-      <c r="AJ7">
-        <v>9.48343</v>
-      </c>
-      <c r="AL7">
-        <v>1.58054</v>
-      </c>
-      <c r="AM7">
-        <v>25.64151</v>
-      </c>
-      <c r="AO7">
-        <v>120.334</v>
-      </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-      <c r="AQ7">
-        <v>34.24801</v>
-      </c>
-      <c r="AR7">
-        <v>5.97099</v>
-      </c>
-      <c r="AS7">
-        <v>67.79949000000001</v>
-      </c>
-      <c r="AT7">
-        <v>105.39804</v>
-      </c>
-      <c r="AU7">
-        <v>97.31551</v>
-      </c>
-      <c r="AV7">
-        <v>52.69182</v>
-      </c>
-      <c r="AW7">
-        <v>49.5299</v>
-      </c>
-      <c r="AX7">
-        <v>102.93811</v>
-      </c>
-      <c r="AY7">
-        <v>61.82655</v>
-      </c>
-      <c r="BA7">
-        <v>21.60186</v>
-      </c>
-      <c r="BB7">
-        <v>70.78603</v>
-      </c>
-      <c r="BC7">
-        <v>1.22931</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2097,7 +1922,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2164,7 +1989,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2">
-        <v>630.188</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0.001724963836062461</v>
@@ -2217,7 +2042,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3">
-        <v>710.104</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0.01952907923740375</v>
@@ -2273,7 +2098,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4">
-        <v>800.131</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0.0107537697827067</v>
@@ -2329,7 +2154,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5">
-        <v>905.029</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0.01060824267020598</v>
@@ -2388,7 +2213,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6">
-        <v>940.061</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0.05236407850460666</v>
@@ -2428,41 +2253,6 @@
       </c>
       <c r="S6">
         <v>0.1630599946910611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7">
-        <v>1000.111</v>
-      </c>
-      <c r="B7">
-        <v>0.3904403477507102</v>
-      </c>
-      <c r="C7">
-        <v>0.5559656730549188</v>
-      </c>
-      <c r="F7">
-        <v>1.141816039754351</v>
-      </c>
-      <c r="I7">
-        <v>0.3337169775271709</v>
-      </c>
-      <c r="J7">
-        <v>0.2616816606866113</v>
-      </c>
-      <c r="N7">
-        <v>1.970314835051048</v>
-      </c>
-      <c r="P7">
-        <v>1.545934469471649</v>
-      </c>
-      <c r="Q7">
-        <v>0.3733519843742963</v>
-      </c>
-      <c r="R7">
-        <v>0.3604795368623867</v>
-      </c>
-      <c r="S7">
-        <v>2.083787280955262</v>
       </c>
     </row>
   </sheetData>
@@ -2472,996 +2262,904 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:55">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:55">
       <c r="A2">
+        <v>630.188</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>-0.0009868510245363523</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.002369456689062963</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.321177658068397</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.334610284186732</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.3346329826127608</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>8.271734338524011</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7.212069606881336</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>10.5908753375122</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>7.064420471035114</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>7.104429508065826</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>6.910254081720142</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>6.72301976646716</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>8.092142994555823</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>6.751293942620885</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>7.069335002800199</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>7.646384411928474</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>5.781068503813306</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>6.251196042384491</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>6.070646474332196</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>5.647660769122093</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>6.36142102139537</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>5.858760701974419</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>2.160652823311019</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>2.194846345568148</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>2.221752221235033</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>2.445671313876951</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>2.494606978787585</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>2.420884934807099</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <v>1.226400344504993</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>1.232453988382594</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>1.237821799711515</v>
       </c>
-      <c r="AN2">
+      <c r="AO2">
         <v>1.285854664692653</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <v>1.256341272787208</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>1.267245336765769</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>0.7169090825445777</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>0.7228491495566002</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <v>0.7030893371885647</v>
       </c>
-      <c r="AT2">
+      <c r="AU2">
         <v>0.7438308805416863</v>
       </c>
-      <c r="AU2">
+      <c r="AV2">
         <v>0.7280710238081137</v>
       </c>
-      <c r="AV2">
+      <c r="AW2">
         <v>0.7319420670612602</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>0.5291258656977472</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <v>0.5297452748983102</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <v>0.5319161883958456</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <v>0.6854918213014732</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>0.6558612851468613</v>
       </c>
-      <c r="BB2">
+      <c r="BC2">
         <v>0.6373295356540289</v>
       </c>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:55">
       <c r="A3">
+        <v>710.104</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.03527755258783717</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.03215688636863803</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.3521547401396932</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.3422254185756777</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.3461522266550301</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>12.27497424921892</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>6.30350266697805</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>6.551219073004707</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9.502349937384105</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>7.225017864312048</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>7.02783389743097</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>6.79837156257643</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>7.7001910655189</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>8.04080832617964</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>9.877047916339993</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>7.880460419087207</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>11.17634297927583</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>7.187274927320402</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>5.565268254081594</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>5.242696790752963</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>4.986055734295956</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>5.213947702742479</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>4.950447934244662</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>5.196917576111406</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>1.858502094329916</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>1.858708955848912</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>1.856642319914637</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>2.066007531363974</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>2.013633823405331</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>2.031369168381267</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>1.103650881377462</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>1.107652578497324</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>1.110470333450653</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>1.15289961092246</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>1.163563588809684</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>1.148779821474097</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>0.6683759443818894</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>0.6610043702662816</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>0.6646834968210266</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>0.6419677404789425</v>
       </c>
-      <c r="AU3">
+      <c r="AV3">
         <v>0.6404484425534448</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>0.6633742292551066</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>0.5014537847257093</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>0.4888927903535583</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>0.4947545510512887</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>0.6368470240465879</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>0.6133229747616171</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>0.5865676943124826</v>
       </c>
     </row>
-    <row r="4" spans="1:54">
+    <row r="4" spans="1:55">
       <c r="A4">
+        <v>800.131</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.02144254092336376</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.01216825791178978</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.3266684479855524</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.3384215441849036</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.3440814590572777</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>6.791067641750565</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>8.070543706253178</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>8.349261066076865</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>8.097943022434288</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>7.831310186146149</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>6.704677473884654</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>5.464640693553923</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>6.704677473884654</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>7.127558030604622</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>5.464640693553923</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>7.538315484663701</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>5.831992439163377</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>6.334273178367257</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>5.201134398847057</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>5.427409397771441</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>4.992757328963292</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>5.26283146579071</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>4.773271159006398</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>5.15760367342838</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>1.865189578994434</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>1.828300269739079</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>1.82840538107907</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>2.09717633028342</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>2.048277982571045</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>2.113581835994198</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>1.053766922316019</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>1.032792623102875</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>1.046057003568155</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>1.071500268853276</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>1.098304388054219</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>1.099722870674653</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>0.612302942770254</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>0.6113415128449541</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>0.6275416624151797</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>0.6280608853753045</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>0.6056226521514031</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>0.6073258119509334</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>0.4714676797787611</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>0.473734774891326</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>0.4557809501659731</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <v>0.5505601740692386</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>0.5358862093517571</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <v>0.5206625184892706</v>
       </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:55">
       <c r="A5">
+        <v>905.029</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>-0.002197188214864343</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.01717662711178382</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.4330045164129592</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.4194023158881378</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.4501551237138702</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>5.084954748651293</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>7.873189521189055</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4.979885428025235</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>6.369080173989713</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>4.800305204556098</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>7.733427455026388</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>5.653909786930866</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>6.31501058852859</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>7.82440111951963</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>10.86895880789553</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>6.106703110172253</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>5.426405771220866</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>5.709794862116025</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>5.151761973549949</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>5.475201074491629</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>4.473393615964602</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>5.606150901558078</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>4.638214755729734</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>2.703027625310849</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>2.930760140926376</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>2.688602283713438</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>2.902551432941729</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>3.014641172775545</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>3.006508210565505</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>1.485825586319976</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>1.516244937192256</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>1.480606853201056</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>1.61734536519812</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>1.599121438917284</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>1.653623857129413</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>0.9548702762228773</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>0.8999113875581437</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>0.9146933478751004</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>0.8517684037259662</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>0.8866381500159414</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>0.909300938432563</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>0.7123219342604135</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>0.7503292663184096</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>0.7191764120959206</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>0.876046724803855</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>0.8159040475761727</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>0.8097464890500682</v>
       </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:55">
       <c r="A6">
+        <v>940.061</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>-0.09135310030747056</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-0.09002684272401879</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.8021053032240173</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.8049390032478694</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.5652512580647395</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2.950981637531783</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3.926144429905822</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>2.954448467996935</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>4.074205015550776</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>4.084900767120548</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>4.539979181535936</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>4.022377200407783</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>3.402521651905551</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>3.140967986227732</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>2.198895888689364</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>2.435234019039055</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>2.331296908075263</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>2.920310762152936</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>7.518939402927136</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>2.519262370349024</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>4.063622453503275</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>2.157344654840557</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>2.111451727002341</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>2.278687789603264</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>1.884949969586585</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>2.053362458677017</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>2.666722014784512</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>2.120463433587223</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>1.498975224973961</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>1.525262779930308</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>1.344507596696353</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>1.351480374278677</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>1.632340245672732</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <v>1.44530619083949</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>1.045232090138032</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>0.9650479096043314</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>1.211327189248919</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>1.232226114806656</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>1.124002912863534</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <v>1.444538029176422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>-0.671928862221308</v>
-      </c>
-      <c r="C7">
-        <v>-0.6805144253648557</v>
-      </c>
-      <c r="D7">
-        <v>-0.3249956860581171</v>
-      </c>
-      <c r="E7">
-        <v>0.7059425900298402</v>
-      </c>
-      <c r="F7">
-        <v>-0.1703148405331999</v>
-      </c>
-      <c r="I7">
-        <v>-0.3158057714911197</v>
-      </c>
-      <c r="L7">
-        <v>-0.06137586178613235</v>
-      </c>
-      <c r="M7">
-        <v>-0.5408314587042193</v>
-      </c>
-      <c r="N7">
-        <v>1.137402760159347</v>
-      </c>
-      <c r="O7">
-        <v>1.63950861351096</v>
-      </c>
-      <c r="Q7">
-        <v>-0.2390797690709351</v>
-      </c>
-      <c r="S7">
-        <v>0.4118516560639531</v>
-      </c>
-      <c r="W7">
-        <v>0.5929122917618943</v>
-      </c>
-      <c r="X7">
-        <v>0.1209652161488118</v>
-      </c>
-      <c r="Y7">
-        <v>-0.493014994593176</v>
-      </c>
-      <c r="Z7">
-        <v>-0.122941241025856</v>
-      </c>
-      <c r="AB7">
-        <v>1.576328019305107</v>
-      </c>
-      <c r="AE7">
-        <v>0.5122773966565201</v>
-      </c>
-      <c r="AI7">
-        <v>1.47916257078485</v>
-      </c>
-      <c r="AK7">
-        <v>3.270942075158769</v>
-      </c>
-      <c r="AL7">
-        <v>0.4844961132846687</v>
-      </c>
-      <c r="AN7">
-        <v>-1.061562573856884</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>91</v>
-      </c>
-      <c r="AP7">
-        <v>0.1950801751282898</v>
-      </c>
-      <c r="AQ7">
-        <v>1.941795893156639</v>
-      </c>
-      <c r="AR7">
-        <v>-0.4878460368354194</v>
-      </c>
-      <c r="AS7">
-        <v>-0.929035404150185</v>
-      </c>
-      <c r="AT7">
-        <v>-0.8492497444352084</v>
-      </c>
-      <c r="AU7">
-        <v>-0.2357515893246583</v>
-      </c>
-      <c r="AV7">
-        <v>-0.1738678916609658</v>
-      </c>
-      <c r="AW7">
-        <v>-0.9054192978874812</v>
-      </c>
-      <c r="AX7">
-        <v>-0.3956242478987219</v>
-      </c>
-      <c r="AZ7">
-        <v>0.6559292138648641</v>
-      </c>
-      <c r="BA7">
-        <v>-0.5309530288873089</v>
-      </c>
-      <c r="BB7">
-        <v>3.522255599589863</v>
       </c>
     </row>
   </sheetData>
@@ -3471,402 +3169,364 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2">
+        <v>630.188</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.3296603191407701</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>7.607194817490235</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>7.728122933146121</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>7.002176291537233</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>6.722559889533247</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>8.091683117621908</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7.090444231679342</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>6.014854420229931</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5.913124903788237</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>2.191644330379332</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2.452793943130414</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1.231754615517668</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1.269279739142317</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.7137883422623288</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.734132323750488</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.5298018505347537</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0.6589046466138117</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
+        <v>710.104</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.3244852376837802</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>6.971752051114541</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>7.181482420175956</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>7.005483339446334</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>7.347239388767625</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>8.423921638456504</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7.839723938535279</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5.214740225814023</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>5.090650467891878</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1.835600133481228</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>2.014417079891322</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1.084903458018339</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1.132711065673662</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.6423328508399366</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.6261915944632312</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.4726699849059673</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>0.5896842798574651</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
+        <v>800.131</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.3251991258713444</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>7.227610240861648</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>8.204562606124053</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>7.820145152460407</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>5.892466341169427</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>6.160749714194783</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>6.339080013451767</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5.180290929122628</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>5.030508234322499</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1.829316559547337</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>2.074793805046334</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1.033002932219159</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1.078592944592312</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.6058695207428427</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.6024528549060915</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.4557975144415266</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.524463430635795</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
+        <v>905.029</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.4291524978073202</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>5.40281683288105</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>5.299282098401393</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>6.22432668209168</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>6.803495292740686</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>6.786384585995152</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>5.553139349503119</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4.938623207221142</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5.004419677264226</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2.763191183787661</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>2.968294235586116</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1.489147027617968</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>1.618152000468391</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.9179340666752709</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.8773329455751595</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.7221838528578617</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>0.8284992157943516</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
+        <v>940.061</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.7789980830304857</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3.385491074810341</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>3.015813041263556</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4.135569588817398</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4.14626534038717</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4.601343754802558</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4.083741773674405</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3.324582366591025</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2.378479853025953</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3.162615780609991</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>2.773284218380979</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>2.139960449682975</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2.306440842563572</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1.514381750740383</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>1.531037263372565</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>1.130052175388308</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>1.319589466339948</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0.4764201009792872</v>
-      </c>
-      <c r="C7">
-        <v>0.1815097644601263</v>
-      </c>
-      <c r="D7">
-        <v>0.4359396741651137</v>
-      </c>
-      <c r="E7">
-        <v>0.7929579290142199</v>
-      </c>
-      <c r="F7">
-        <v>0.2582357668803111</v>
-      </c>
-      <c r="G7">
-        <v>0.9091671920151991</v>
-      </c>
-      <c r="H7">
-        <v>0.8266671493369104</v>
-      </c>
-      <c r="I7">
-        <v>0.1723149028879223</v>
-      </c>
-      <c r="J7">
-        <v>2.073643555256353</v>
-      </c>
-      <c r="K7">
-        <v>1.009592932607766</v>
-      </c>
-      <c r="L7">
-        <v>1.976478106736096</v>
-      </c>
-      <c r="M7">
-        <v>1.615144045812054</v>
-      </c>
-      <c r="N7">
-        <v>0.2839116960081089</v>
-      </c>
-      <c r="O7">
-        <v>0.1363096451118474</v>
-      </c>
-      <c r="P7">
-        <v>0.02863562511753045</v>
-      </c>
-      <c r="Q7">
-        <v>-0.1853468002619424</v>
-      </c>
-      <c r="R7">
-        <v>0.7854223332927206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>